<commit_message>
started parsing of gas mixing sheet
</commit_message>
<xml_diff>
--- a/tests/data/2023_06_12/MBE8_config.xlsx
+++ b/tests/data/2023_06_12/MBE8_config.xlsx
@@ -122,52 +122,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Bierwagen:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">pick from substrate_range/growers</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Bierwagen:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">pick from substrate_range/growers</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -268,7 +222,7 @@
     <t xml:space="preserve"># format</t>
   </si>
   <si>
-    <t xml:space="preserve">dd.mm.yyyy</t>
+    <t xml:space="preserve">dd/mm/yyyy</t>
   </si>
   <si>
     <t xml:space="preserve">hh:mm:ss</t>
@@ -358,7 +312,7 @@
     <t xml:space="preserve">r power unit</t>
   </si>
   <si>
-    <t xml:space="preserve">02.11.23</t>
+    <t xml:space="preserve">02/11/2023</t>
   </si>
   <si>
     <t xml:space="preserve">08:59:00</t>
@@ -502,28 +456,22 @@
     <t xml:space="preserve">mfc serial number</t>
   </si>
   <si>
-    <t xml:space="preserve">mfc1_range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc1_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc1_gas_provenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc1_flow_EPIC_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc2_range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc2_gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc2_gas_provenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mfc2_flow_EPIC_name</t>
+    <t xml:space="preserve">mfc_range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfc_gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfc_gas_provenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfc_flow_EPIC_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/06/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">GH</t>
@@ -545,6 +493,12 @@
   </si>
   <si>
     <t xml:space="preserve">N.MF.MV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/06/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08:45:00</t>
   </si>
   <si>
     <t xml:space="preserve">AA</t>
@@ -619,7 +573,7 @@
     <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="172" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -677,6 +631,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -818,7 +778,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1007,6 +967,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1027,6 +991,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1059,6 +1027,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1071,6 +1043,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1087,11 +1063,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1430,14 +1406,14 @@
   </sheetPr>
   <dimension ref="A1:AV49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC14" activeCellId="0" sqref="AC14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="13.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="13.15"/>
@@ -2657,35 +2633,34 @@
   <dimension ref="A1:AP35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="15.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="47" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="47" width="13.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="47" width="13.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="47" width="11.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="47" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="47" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="47" width="13.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="47" width="18.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="47" width="21.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="47" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="47" width="5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="16" style="47" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="48" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="13.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="48" width="19.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="48" width="13.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="48" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="48" width="21.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="48" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="48" width="5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="38" min="12" style="48" width="10.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16380" min="43" style="48" width="10.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16381" style="48" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="50" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="51" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -2698,50 +2673,48 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="49" t="s">
         <v>102</v>
       </c>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="48" t="s">
-        <v>102</v>
-      </c>
+      <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
+      <c r="Q1" s="50"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="49"/>
+      <c r="U1" s="6"/>
       <c r="V1" s="6"/>
       <c r="W1" s="6"/>
       <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="8"/>
       <c r="AA1" s="6"/>
       <c r="AB1" s="6"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="8"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="6"/>
       <c r="AE1" s="6"/>
       <c r="AF1" s="6"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
+      <c r="AG1" s="6"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
       <c r="AK1" s="6"/>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-    </row>
-    <row r="2" s="51" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL1" s="6"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
+      <c r="AO1" s="0"/>
+      <c r="AP1" s="0"/>
+    </row>
+    <row r="2" s="52" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -2753,12 +2726,8 @@
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>104</v>
-      </c>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="N2" s="13"/>
       <c r="O2" s="13"/>
@@ -2771,36 +2740,36 @@
       <c r="V2" s="13"/>
       <c r="W2" s="13"/>
       <c r="X2" s="13"/>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="15"/>
       <c r="AA2" s="13"/>
       <c r="AB2" s="13"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="15"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="13"/>
       <c r="AE2" s="13"/>
       <c r="AF2" s="13"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-      <c r="AJ2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="17"/>
       <c r="AK2" s="13"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="17"/>
-      <c r="AN2" s="17"/>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="13"/>
-    </row>
-    <row r="3" s="53" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+    </row>
+    <row r="3" s="55" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="54" t="s">
         <v>105</v>
       </c>
       <c r="E3" s="20"/>
@@ -2809,50 +2778,50 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
-      <c r="R3" s="52"/>
-      <c r="S3" s="52"/>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="V3" s="52"/>
-      <c r="W3" s="52"/>
-      <c r="X3" s="52"/>
-      <c r="Y3" s="52"/>
-      <c r="Z3" s="52"/>
-      <c r="AA3" s="52"/>
-      <c r="AB3" s="52"/>
-      <c r="AC3" s="52"/>
-      <c r="AD3" s="52"/>
-      <c r="AE3" s="52"/>
-      <c r="AF3" s="52"/>
-      <c r="AG3" s="52"/>
-      <c r="AH3" s="52"/>
-      <c r="AI3" s="52"/>
-      <c r="AJ3" s="52"/>
-      <c r="AK3" s="52"/>
-      <c r="AL3" s="52"/>
-      <c r="AM3" s="52"/>
-      <c r="AN3" s="52"/>
-      <c r="AO3" s="52"/>
-      <c r="AP3" s="52"/>
-    </row>
-    <row r="4" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54"/>
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="54"/>
+      <c r="AG3" s="54"/>
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="54"/>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54"/>
+      <c r="AL3" s="54"/>
+      <c r="AM3" s="0"/>
+      <c r="AN3" s="0"/>
+      <c r="AO3" s="0"/>
+      <c r="AP3" s="0"/>
+    </row>
+    <row r="4" s="61" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="56" t="s">
         <v>106</v>
       </c>
       <c r="E4" s="28"/>
@@ -2875,99 +2844,93 @@
       <c r="V4" s="28"/>
       <c r="W4" s="28"/>
       <c r="X4" s="28"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="58"/>
       <c r="AA4" s="28"/>
       <c r="AB4" s="28"/>
-      <c r="AC4" s="55"/>
-      <c r="AD4" s="56"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="28"/>
       <c r="AE4" s="28"/>
       <c r="AF4" s="28"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="28"/>
-      <c r="AI4" s="28"/>
-      <c r="AJ4" s="28"/>
+      <c r="AG4" s="28"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="60"/>
+      <c r="AJ4" s="60"/>
       <c r="AK4" s="28"/>
-      <c r="AL4" s="55"/>
-      <c r="AM4" s="58"/>
-      <c r="AN4" s="58"/>
-      <c r="AO4" s="28"/>
-      <c r="AP4" s="28"/>
-    </row>
-    <row r="5" s="50" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL4" s="28"/>
+      <c r="AM4" s="0"/>
+      <c r="AN4" s="0"/>
+      <c r="AO4" s="0"/>
+      <c r="AP4" s="0"/>
+    </row>
+    <row r="5" s="51" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="60" t="s">
+      <c r="H5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="60" t="s">
+      <c r="I5" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="60" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="60"/>
-      <c r="W5" s="60"/>
-      <c r="X5" s="60"/>
-      <c r="Y5" s="60"/>
-      <c r="Z5" s="60"/>
-      <c r="AA5" s="60"/>
-      <c r="AB5" s="60"/>
-      <c r="AC5" s="60"/>
-      <c r="AD5" s="61"/>
-      <c r="AE5" s="61"/>
-      <c r="AF5" s="61"/>
-      <c r="AG5" s="61"/>
-      <c r="AH5" s="61"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="61"/>
-      <c r="AK5" s="61"/>
-      <c r="AL5" s="61"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="61"/>
-      <c r="AP5" s="61"/>
-    </row>
-    <row r="6" s="62" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="64"/>
+      <c r="AA5" s="64"/>
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="64"/>
+      <c r="AI5" s="64"/>
+      <c r="AJ5" s="64"/>
+      <c r="AK5" s="64"/>
+      <c r="AL5" s="64"/>
+      <c r="AM5" s="0"/>
+      <c r="AN5" s="0"/>
+      <c r="AO5" s="0"/>
+      <c r="AP5" s="0"/>
+    </row>
+    <row r="6" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="34" t="s">
@@ -2992,20 +2955,12 @@
         <v>112</v>
       </c>
       <c r="K6" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="L6" s="34" t="s">
-        <v>114</v>
-      </c>
-      <c r="M6" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="N6" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="O6" s="34" t="s">
         <v>12</v>
       </c>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="34"/>
       <c r="Q6" s="34"/>
       <c r="R6" s="34"/>
@@ -3015,308 +2970,297 @@
       <c r="V6" s="34"/>
       <c r="W6" s="34"/>
       <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
+      <c r="Y6" s="35"/>
+      <c r="Z6" s="36"/>
       <c r="AA6" s="34"/>
       <c r="AB6" s="34"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="36"/>
+      <c r="AC6" s="37"/>
+      <c r="AD6" s="34"/>
       <c r="AE6" s="34"/>
       <c r="AF6" s="34"/>
-      <c r="AG6" s="37"/>
-      <c r="AH6" s="34"/>
-      <c r="AI6" s="34"/>
-      <c r="AJ6" s="34"/>
+      <c r="AG6" s="34"/>
+      <c r="AH6" s="35"/>
+      <c r="AI6" s="38"/>
+      <c r="AJ6" s="38"/>
       <c r="AK6" s="34"/>
-      <c r="AL6" s="35"/>
-      <c r="AM6" s="38"/>
-      <c r="AN6" s="38"/>
-      <c r="AO6" s="34"/>
-      <c r="AP6" s="34"/>
+      <c r="AL6" s="34"/>
+      <c r="AM6" s="0"/>
+      <c r="AN6" s="0"/>
+      <c r="AO6" s="0"/>
+      <c r="AP6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="63" t="s">
+      <c r="B7" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="47" t="n">
+      <c r="I7" s="68"/>
+      <c r="J7" s="68" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="68" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
+      <c r="T7" s="68"/>
+      <c r="U7" s="68"/>
+      <c r="V7" s="68"/>
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="68" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="68"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="47" t="s">
+      <c r="H9" s="68" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64" t="s">
-        <v>120</v>
-      </c>
-      <c r="O7" s="64" t="s">
+      <c r="K9" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="69"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="72"/>
+      <c r="H10" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="65"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="H8" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="66" t="s">
-        <v>123</v>
-      </c>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="64"/>
-      <c r="T8" s="65"/>
-      <c r="U8" s="64"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="F9" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="64"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="64"/>
-      <c r="N9" s="66"/>
-      <c r="O9" s="47" t="s">
-        <v>125</v>
-      </c>
-      <c r="Q9" s="68"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="68"/>
-      <c r="T9" s="65"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="67"/>
-      <c r="H10" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="J10" s="66"/>
-      <c r="K10" s="64"/>
-      <c r="M10" s="66"/>
-      <c r="Q10" s="68"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="68"/>
-      <c r="T10" s="65"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="69"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="64"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="67"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="64"/>
-      <c r="M11" s="66"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="68"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="65"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="L11" s="71"/>
+      <c r="M11" s="71"/>
+      <c r="N11" s="71"/>
+      <c r="O11" s="69"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G12" s="64"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="67"/>
-      <c r="J12" s="67"/>
-      <c r="K12" s="64"/>
-      <c r="M12" s="66"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="65"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="72"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="69"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G13" s="64"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="64"/>
-      <c r="M13" s="66"/>
-      <c r="P13" s="68"/>
-      <c r="Q13" s="68"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="65"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="72"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
+      <c r="O13" s="69"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G14" s="64"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="M14" s="66"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="68"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="65"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="72"/>
+      <c r="L14" s="71"/>
+      <c r="M14" s="71"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="69"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G15" s="64"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="M15" s="66"/>
+      <c r="G15" s="68"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="64"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="M16" s="66"/>
-      <c r="S16" s="65"/>
+      <c r="G16" s="68"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="72"/>
+      <c r="O16" s="69"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="64"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="M17" s="66"/>
-      <c r="S17" s="65"/>
+      <c r="G17" s="68"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="72"/>
+      <c r="O17" s="69"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="64"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="M18" s="66"/>
-      <c r="R18" s="68"/>
-      <c r="S18" s="65"/>
+      <c r="G18" s="68"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="69"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G19" s="64"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="M19" s="66"/>
-      <c r="S19" s="65"/>
-      <c r="AA19" s="70"/>
+      <c r="G19" s="68"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="O19" s="69"/>
+      <c r="W19" s="74"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="S20" s="65"/>
+      <c r="I20" s="72"/>
+      <c r="J20" s="72"/>
+      <c r="O20" s="69"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="S21" s="65"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="O21" s="69"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="S22" s="65"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="O22" s="69"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="65"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="69"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="S24" s="65"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="O24" s="69"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="S25" s="65"/>
+      <c r="I25" s="72"/>
+      <c r="J25" s="72"/>
+      <c r="O25" s="69"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="S26" s="65"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="O26" s="69"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="S27" s="65"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="72"/>
+      <c r="O27" s="69"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="S28" s="65"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="72"/>
+      <c r="O28" s="69"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="S29" s="65"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
+      <c r="O29" s="69"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="S30" s="65"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="72"/>
+      <c r="O30" s="69"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="S31" s="65"/>
+      <c r="I31" s="72"/>
+      <c r="J31" s="72"/>
+      <c r="O31" s="69"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="S32" s="65"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="O32" s="69"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3324,7 +3268,7 @@
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="T7:T10 S11:S14 S16:S32" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="P7:P10 O11:O14 O16:O32" type="list">
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3332,7 +3276,7 @@
       <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H7:H10 L9 K10:K13 G11:G12" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H7:H10 G11:G12" type="list">
       <formula1>'MBE config ranges'!$C$7:$C$11</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3370,119 +3314,119 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="3" width="10.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="49" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="50" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="71"/>
-    </row>
-    <row r="2" s="73" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="72" t="s">
+      <c r="J1" s="75"/>
+    </row>
+    <row r="2" s="77" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="74"/>
-    </row>
-    <row r="3" s="53" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J2" s="78"/>
+    </row>
+    <row r="3" s="55" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="75"/>
-    </row>
-    <row r="4" s="59" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="79"/>
+    </row>
+    <row r="4" s="61" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="76"/>
-    </row>
-    <row r="5" s="78" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="77" t="s">
+      <c r="J4" s="80"/>
+    </row>
+    <row r="5" s="82" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="79"/>
+      <c r="J5" s="83"/>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="82" t="s">
+      <c r="B6" s="85"/>
+      <c r="C6" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="86" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="83" t="s">
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="84" t="s">
+      <c r="D7" s="88" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="88" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="88" t="s">
         <v>126</v>
       </c>
-      <c r="D8" s="84" t="s">
+      <c r="D8" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="84" t="s">
+      <c r="J8" s="88" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="84" t="s">
+      <c r="K8" s="88" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="84" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="84" t="s">
+      <c r="C9" s="88" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="88" t="s">
         <v>85</v>
       </c>
-      <c r="J9" s="84" t="s">
+      <c r="J9" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="84" t="s">
+      <c r="K9" s="88" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="88" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="84" t="s">
+      <c r="D10" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="J10" s="84" t="s">
+      <c r="J10" s="88" t="s">
         <v>133</v>
       </c>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="88" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J11" s="84" t="s">
+      <c r="J11" s="88" t="s">
         <v>97</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="88" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3514,39 +3458,39 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="true" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="49" customFormat="true" ht="46.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" s="51" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="52" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" s="53" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="55" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="61" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" s="78" customFormat="true" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="77" t="s">
+    <row r="5" s="82" customFormat="true" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="81" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" s="62" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
+    <row r="6" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="65" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3579,57 +3523,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="85" width="14.06"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="86" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="89" width="14.06"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="2" style="90" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="49" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="91" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" s="52" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="54" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="88" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="92" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" s="89" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="77" t="s">
+    <row r="5" s="93" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="81" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" s="62" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="62" t="s">
+    <row r="6" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="65" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="65" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="90" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>